<commit_message>
UPDATE import_users.php ADD asignarSeccion.php
</commit_message>
<xml_diff>
--- a/excel/usuarios.xlsx
+++ b/excel/usuarios.xlsx
@@ -11,18 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
-  <si>
-    <t>CORREO</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Bonilla@evg</t>
   </si>
@@ -202,7 +196,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -213,12 +207,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -256,7 +244,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -264,40 +252,25 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color indexed="8"/>
-      </left>
-      <right style="hair">
-        <color indexed="8"/>
-      </right>
-      <top style="hair">
-        <color indexed="8"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="3"/>
@@ -663,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -675,245 +648,276 @@
     <col min="2" max="2" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="2" t="s">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="2" t="s">
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" ht="15">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15">
-      <c r="A17" s="2" t="s">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" ht="15">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15">
-      <c r="A18" s="2" t="s">
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" ht="15">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15">
-      <c r="A19" s="2" t="s">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="15">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15">
-      <c r="A20" s="2" t="s">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" ht="15">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15">
-      <c r="A21" s="2" t="s">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" ht="15">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15">
-      <c r="A22" s="2" t="s">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" ht="15">
+      <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15">
-      <c r="A23" s="2" t="s">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" ht="15">
+      <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15">
-      <c r="A24" s="2" t="s">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" ht="15">
+      <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15">
-      <c r="A25" s="2" t="s">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" ht="15">
+      <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15">
-      <c r="A26" s="2" t="s">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" ht="15">
+      <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15">
-      <c r="A27" s="2" t="s">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" ht="15">
+      <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="15">
-      <c r="A28" s="2" t="s">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" ht="15">
+      <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="15">
-      <c r="A29" s="2" t="s">
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75">
+      <c r="A29" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75">
-      <c r="A30" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>59</v>
-      </c>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.75">
+      <c r="A30" s="5"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
UPDATE: Quitar tablas "fantasma" de usuarios.xslx y ciertos arreglos
</commit_message>
<xml_diff>
--- a/excel/usuarios.xlsx
+++ b/excel/usuarios.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampisapaco\htdocs\Incidencias_EVG\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="194"/>
   </bookViews>
@@ -195,8 +200,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -348,6 +353,14 @@
       <rgbColor rgb="00424242"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -394,7 +407,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -426,9 +439,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -460,6 +474,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -635,20 +650,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +672,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -666,7 +681,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -675,7 +690,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -684,7 +699,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -693,7 +708,7 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -702,7 +717,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -711,7 +726,7 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -720,7 +735,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -729,7 +744,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -738,7 +753,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -747,7 +762,7 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -756,7 +771,7 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -765,7 +780,7 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -774,7 +789,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -783,7 +798,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" ht="15">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -792,7 +807,7 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" ht="15">
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -801,7 +816,7 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -810,7 +825,7 @@
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" ht="15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -819,7 +834,7 @@
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -828,7 +843,7 @@
       </c>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" ht="15">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -837,7 +852,7 @@
       </c>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" ht="15">
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -846,7 +861,7 @@
       </c>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" ht="15">
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -855,7 +870,7 @@
       </c>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" ht="15">
+    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -864,7 +879,7 @@
       </c>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" ht="15">
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -873,7 +888,7 @@
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" ht="15">
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -882,7 +897,7 @@
       </c>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" ht="15">
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -891,7 +906,7 @@
       </c>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" ht="15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
@@ -900,7 +915,7 @@
       </c>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" ht="15.75">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>56</v>
       </c>
@@ -908,16 +923,6 @@
         <v>57</v>
       </c>
       <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" ht="15.75">
-      <c r="A30" s="5"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -930,12 +935,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -947,12 +952,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>